<commit_message>
ANN methodology and ANN performance tables updated
</commit_message>
<xml_diff>
--- a/Chapters/05_Artificial_Neural_Networks_for_EHL_Film_Thickness_Predictions/Rsquared and Time Performance of ANNs.xlsx
+++ b/Chapters/05_Artificial_Neural_Networks_for_EHL_Film_Thickness_Predictions/Rsquared and Time Performance of ANNs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunet-my.sharepoint.com/personal/wshq_lunet_lboro_ac_uk/Documents/PhD R1/11.0 Thesis/Chapters/05_Artificial_Neural_Networks_for_EHL_Film_Thickness_Predictions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\PhDThesis\Chapters\05_Artificial_Neural_Networks_for_EHL_Film_Thickness_Predictions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{A88CE0D1-3193-44A7-BEDD-E2D405024EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97242F15-B576-48BE-8F7A-B3AC1DD1152E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA47B074-C462-4448-AEFE-00FCC0E29EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{FC869EDD-D144-4FFB-83F7-A05B0BA9D432}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC869EDD-D144-4FFB-83F7-A05B0BA9D432}"/>
   </bookViews>
   <sheets>
     <sheet name="Rsquared" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>R²</t>
   </si>
@@ -166,8 +169,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -231,7 +235,7 @@
       <name val="Serif"/>
     </font>
   </fonts>
-  <fills count="127">
+  <fills count="171">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,12 +388,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFCBE7B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF71C27C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -450,12 +448,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC1DA81"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF83C87D"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -985,6 +977,282 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB1D580"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEE983"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA0D07F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDD780"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9CCF7F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8BCA7E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD480"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF88C97E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5D17F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E483"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAAD380"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E082"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0E283"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCB77A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDD880"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF80C77D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBA777"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE182"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEE683"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA9D75"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDD47F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCEDD82"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8D780"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA9874"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDD17F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8766D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF86E6B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF97E6F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDC77D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCBF7B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBB078"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDCF7E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA9573"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFED980"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEE582"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8736D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCB87A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8E583"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBAF78"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA9974"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBB279"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA9273"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBA376"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA9F75"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8716C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDD07E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1403,7 +1671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="250">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1471,6 +1739,9 @@
     <xf numFmtId="164" fontId="5" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="26" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1495,10 +1766,13 @@
     <xf numFmtId="164" fontId="5" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="40" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="41" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="42" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1514,21 +1788,21 @@
     <xf numFmtId="2" fontId="5" fillId="46" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="47" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="48" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="49" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="48" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="49" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="50" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1547,54 +1821,54 @@
     <xf numFmtId="2" fontId="5" fillId="55" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="57" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="58" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="59" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="60" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="61" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="65" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="67" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="68" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="69" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="70" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="71" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="73" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="74" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="56" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="57" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="59" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="60" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="61" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="62" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="63" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="67" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="69" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="70" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="71" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="72" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="73" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="75" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="76" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="58" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="77" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1619,12 +1893,12 @@
     <xf numFmtId="2" fontId="5" fillId="84" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="85" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="86" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="87" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="88" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1670,10 +1944,10 @@
     <xf numFmtId="2" fontId="5" fillId="102" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="103" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="104" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="109" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="110" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="111" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1712,42 +1986,36 @@
     <xf numFmtId="2" fontId="5" fillId="122" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="123" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="124" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="104" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="97" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="99" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="102" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="56" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="101" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="105" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="106" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="99" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="101" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="104" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="58" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="103" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="107" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="108" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="109" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="110" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1763,79 +2031,91 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="58" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="85" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="105" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="56" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="83" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="103" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="41" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="39" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="58" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="56" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="65" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="63" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="14" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="74" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="82" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="80" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="72" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="80" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="78" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="23" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="83" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="84" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="82" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="5" fillId="85" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="86" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="84" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="87" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="88" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="89" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="112" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="125" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="76" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="80" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="87" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="110" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="123" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="74" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="78" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="16" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="57" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="64" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="55" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="62" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="64" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="65" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="59" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="57" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="66" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1844,74 +2124,14 @@
     <xf numFmtId="2" fontId="5" fillId="67" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="61" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="59" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="68" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="69" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="56" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="60" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="50" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="25" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="36" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="31" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="38" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="39" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="40" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="28" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="14" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="14" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="26" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="37" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="41" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="5" fillId="54" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="58" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="48" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1922,34 +2142,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="126" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="126" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="126" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="124" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="124" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="124" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="126" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="126" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="126" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="126" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="124" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="124" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="124" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="124" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1961,49 +2181,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="126" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2021,8 +2220,203 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="124" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="25" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="38" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="125" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="126" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="127" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="128" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="129" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="130" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="131" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="132" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="133" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="134" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="135" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="136" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="137" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="138" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="139" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="140" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="141" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="142" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="143" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="144" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="145" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="146" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="147" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="148" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="149" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="150" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="151" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="152" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="153" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="154" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="155" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="156" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="157" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="158" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="159" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="160" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="161" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="162" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="163" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="164" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="165" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="166" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="167" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="168" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="169" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="164" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="170" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="39" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2030,6 +2424,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF63BE7B"/>
+      <color rgb="FFF8696B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2041,14 +2441,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2086,7 +2482,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2192,7 +2588,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2334,7 +2730,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2344,18 +2740,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AEA055-F48F-410E-BD80-769AA7F315FA}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N2"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.68359375" customWidth="1"/>
-    <col min="15" max="15" width="3.83984375" customWidth="1"/>
-    <col min="16" max="16" width="9.15625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="3.85546875" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.7" thickBot="1">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1">
       <c r="A1" s="32"/>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -2375,58 +2771,58 @@
       <c r="Q1" s="32"/>
       <c r="R1" s="32"/>
     </row>
-    <row r="2" spans="1:18" ht="28" customHeight="1" thickBot="1">
+    <row r="2" spans="1:18" ht="27.95" customHeight="1" thickBot="1">
       <c r="A2" s="32"/>
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="158" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175"/>
-      <c r="N2" s="176"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="160"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="177" t="s">
+      <c r="P2" s="161" t="s">
         <v>12</v>
       </c>
       <c r="Q2" s="32"/>
       <c r="R2" s="32"/>
     </row>
-    <row r="3" spans="1:18" ht="14.7" thickBot="1">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1">
       <c r="A3" s="32"/>
-      <c r="B3" s="180" t="s">
+      <c r="B3" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="184" t="s">
+      <c r="C3" s="165"/>
+      <c r="D3" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="185"/>
-      <c r="L3" s="185"/>
-      <c r="M3" s="185"/>
-      <c r="N3" s="186"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
+      <c r="L3" s="169"/>
+      <c r="M3" s="169"/>
+      <c r="N3" s="170"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="178"/>
+      <c r="P3" s="162"/>
       <c r="Q3" s="32"/>
       <c r="R3" s="32"/>
     </row>
-    <row r="4" spans="1:18" ht="14.7" thickBot="1">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1">
       <c r="A4" s="32"/>
-      <c r="B4" s="182"/>
-      <c r="C4" s="183"/>
+      <c r="B4" s="166"/>
+      <c r="C4" s="167"/>
       <c r="D4" s="118">
         <v>10</v>
       </c>
@@ -2461,13 +2857,13 @@
         <v>20</v>
       </c>
       <c r="O4" s="1"/>
-      <c r="P4" s="179"/>
+      <c r="P4" s="162"/>
       <c r="Q4" s="32"/>
       <c r="R4" s="32"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
       <c r="A5" s="32"/>
-      <c r="B5" s="171" t="s">
+      <c r="B5" s="155" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="118">
@@ -2503,11 +2899,11 @@
       <c r="M5" s="12">
         <v>0.995</v>
       </c>
-      <c r="N5" s="155">
+      <c r="N5" s="193">
         <v>0.999</v>
       </c>
-      <c r="O5" s="2"/>
-      <c r="P5" s="167">
+      <c r="O5" s="192"/>
+      <c r="P5" s="245">
         <v>0.99</v>
       </c>
       <c r="Q5" s="32"/>
@@ -2515,7 +2911,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="32"/>
-      <c r="B6" s="172"/>
+      <c r="B6" s="156"/>
       <c r="C6" s="116">
         <v>2</v>
       </c>
@@ -2549,11 +2945,11 @@
       <c r="M6" s="22">
         <v>0.997</v>
       </c>
-      <c r="N6" s="156">
+      <c r="N6" s="194">
         <v>0.995</v>
       </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="168">
+      <c r="O6" s="192"/>
+      <c r="P6" s="246">
         <v>0.99299999999999999</v>
       </c>
       <c r="Q6" s="32"/>
@@ -2561,7 +2957,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="32"/>
-      <c r="B7" s="172"/>
+      <c r="B7" s="156"/>
       <c r="C7" s="116">
         <v>3</v>
       </c>
@@ -2595,57 +2991,57 @@
       <c r="M7" s="31">
         <v>0.995</v>
       </c>
-      <c r="N7" s="157">
+      <c r="N7" s="195">
         <v>0.996</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="169">
+      <c r="O7" s="192"/>
+      <c r="P7" s="247">
         <v>0.997</v>
       </c>
       <c r="Q7" s="32"/>
       <c r="R7" s="32"/>
     </row>
-    <row r="8" spans="1:18" ht="14.7" thickBot="1">
+    <row r="8" spans="1:18" ht="15.75" thickBot="1">
       <c r="A8" s="32"/>
-      <c r="B8" s="173"/>
+      <c r="B8" s="157"/>
       <c r="C8" s="119">
         <v>4</v>
       </c>
-      <c r="D8" s="158">
+      <c r="D8" s="27">
         <v>0.997</v>
       </c>
-      <c r="E8" s="159">
+      <c r="E8" s="196">
         <v>0.999</v>
       </c>
-      <c r="F8" s="160">
+      <c r="F8" s="197">
         <v>0.997</v>
       </c>
-      <c r="G8" s="161">
+      <c r="G8" s="3">
         <v>0.997</v>
       </c>
-      <c r="H8" s="162">
+      <c r="H8" s="198">
         <v>0.999</v>
       </c>
-      <c r="I8" s="163">
+      <c r="I8" s="24">
         <v>0.998</v>
       </c>
-      <c r="J8" s="164">
+      <c r="J8" s="30">
         <v>0.99299999999999999</v>
       </c>
-      <c r="K8" s="165">
+      <c r="K8" s="199">
         <v>0.98899999999999999</v>
       </c>
-      <c r="L8" s="165">
+      <c r="L8" s="199">
         <v>0.98899999999999999</v>
       </c>
-      <c r="M8" s="165">
+      <c r="M8" s="199">
         <v>0.97499999999999998</v>
       </c>
-      <c r="N8" s="166">
+      <c r="N8" s="199">
         <v>0.99</v>
       </c>
-      <c r="O8" s="2"/>
-      <c r="P8" s="170">
+      <c r="O8" s="192"/>
+      <c r="P8" s="248">
         <v>1</v>
       </c>
       <c r="Q8" s="32"/>
@@ -2671,7 +3067,7 @@
       <c r="Q9" s="32"/>
       <c r="R9" s="32"/>
     </row>
-    <row r="10" spans="1:18" ht="14.7" thickBot="1">
+    <row r="10" spans="1:18" ht="15.75" thickBot="1">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
@@ -2691,58 +3087,58 @@
       <c r="Q10" s="32"/>
       <c r="R10" s="32"/>
     </row>
-    <row r="11" spans="1:18" ht="28" customHeight="1" thickBot="1">
+    <row r="11" spans="1:18" ht="27.95" customHeight="1" thickBot="1">
       <c r="A11" s="32"/>
-      <c r="B11" s="174" t="s">
+      <c r="B11" s="158" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="175"/>
-      <c r="D11" s="175"/>
-      <c r="E11" s="175"/>
-      <c r="F11" s="175"/>
-      <c r="G11" s="175"/>
-      <c r="H11" s="175"/>
-      <c r="I11" s="175"/>
-      <c r="J11" s="175"/>
-      <c r="K11" s="175"/>
-      <c r="L11" s="175"/>
-      <c r="M11" s="175"/>
-      <c r="N11" s="176"/>
+      <c r="C11" s="159"/>
+      <c r="D11" s="159"/>
+      <c r="E11" s="159"/>
+      <c r="F11" s="159"/>
+      <c r="G11" s="159"/>
+      <c r="H11" s="159"/>
+      <c r="I11" s="159"/>
+      <c r="J11" s="159"/>
+      <c r="K11" s="159"/>
+      <c r="L11" s="159"/>
+      <c r="M11" s="159"/>
+      <c r="N11" s="160"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="177" t="s">
+      <c r="P11" s="161" t="s">
         <v>11</v>
       </c>
       <c r="Q11" s="32"/>
       <c r="R11" s="32"/>
     </row>
-    <row r="12" spans="1:18" ht="14.7" thickBot="1">
+    <row r="12" spans="1:18" ht="15.75" thickBot="1">
       <c r="A12" s="32"/>
-      <c r="B12" s="180" t="s">
+      <c r="B12" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="181"/>
-      <c r="D12" s="184" t="s">
+      <c r="C12" s="165"/>
+      <c r="D12" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="185"/>
-      <c r="F12" s="185"/>
-      <c r="G12" s="185"/>
-      <c r="H12" s="185"/>
-      <c r="I12" s="185"/>
-      <c r="J12" s="185"/>
-      <c r="K12" s="185"/>
-      <c r="L12" s="185"/>
-      <c r="M12" s="185"/>
-      <c r="N12" s="186"/>
+      <c r="E12" s="169"/>
+      <c r="F12" s="169"/>
+      <c r="G12" s="169"/>
+      <c r="H12" s="169"/>
+      <c r="I12" s="169"/>
+      <c r="J12" s="169"/>
+      <c r="K12" s="169"/>
+      <c r="L12" s="169"/>
+      <c r="M12" s="169"/>
+      <c r="N12" s="170"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="178"/>
+      <c r="P12" s="162"/>
       <c r="Q12" s="32"/>
       <c r="R12" s="32"/>
     </row>
-    <row r="13" spans="1:18" ht="14.7" thickBot="1">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1">
       <c r="A13" s="32"/>
-      <c r="B13" s="182"/>
-      <c r="C13" s="183"/>
+      <c r="B13" s="166"/>
+      <c r="C13" s="167"/>
       <c r="D13" s="118">
         <v>10</v>
       </c>
@@ -2777,53 +3173,53 @@
         <v>20</v>
       </c>
       <c r="O13" s="1"/>
-      <c r="P13" s="179"/>
+      <c r="P13" s="162"/>
       <c r="Q13" s="32"/>
       <c r="R13" s="32"/>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
       <c r="A14" s="32"/>
-      <c r="B14" s="171" t="s">
+      <c r="B14" s="155" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="118">
         <v>1</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="200">
         <v>0.998</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="8">
         <v>0.999</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="201">
         <v>0.995</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="202">
         <v>0.998</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <v>0.998</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="203">
         <v>0.99399999999999999</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="204">
         <v>0.998</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="205">
         <v>0.999</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="204">
         <v>0.998</v>
       </c>
-      <c r="M14" s="12">
+      <c r="M14" s="206">
         <v>0.998</v>
       </c>
-      <c r="N14" s="155">
+      <c r="N14" s="6">
         <v>0.998</v>
       </c>
-      <c r="O14" s="2"/>
-      <c r="P14" s="167">
+      <c r="O14" s="192"/>
+      <c r="P14" s="245">
         <v>0.99</v>
       </c>
       <c r="Q14" s="32"/>
@@ -2831,45 +3227,45 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="32"/>
-      <c r="B15" s="172"/>
+      <c r="B15" s="156"/>
       <c r="C15" s="116">
         <v>2</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="207">
         <v>0.999</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="208">
         <v>0.998</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="24">
         <v>0.998</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="196">
         <v>0.999</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="209">
         <v>0.996</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="210">
         <v>0.998</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="211">
         <v>0.996</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K15" s="209">
         <v>0.996</v>
       </c>
-      <c r="L15" s="21">
+      <c r="L15" s="212">
         <v>0.996</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="213">
         <v>0.99299999999999999</v>
       </c>
-      <c r="N15" s="156">
+      <c r="N15" s="214">
         <v>0.99399999999999999</v>
       </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="168">
+      <c r="O15" s="192"/>
+      <c r="P15" s="246">
         <v>0.99299999999999999</v>
       </c>
       <c r="Q15" s="32"/>
@@ -2877,91 +3273,91 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="32"/>
-      <c r="B16" s="172"/>
+      <c r="B16" s="156"/>
       <c r="C16" s="116">
         <v>3</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="215">
         <v>0.999</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="216">
         <v>0.99199999999999999</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="217">
         <v>0.996</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="218">
         <v>0.995</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="219">
         <v>0.99199999999999999</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="199">
         <v>0.98899999999999999</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="199">
         <v>0.98899999999999999</v>
       </c>
-      <c r="K16" s="29">
+      <c r="K16" s="199">
         <v>0.98499999999999999</v>
       </c>
-      <c r="L16" s="30">
+      <c r="L16" s="220">
         <v>0.99399999999999999</v>
       </c>
-      <c r="M16" s="31">
+      <c r="M16" s="199">
         <v>0.97</v>
       </c>
-      <c r="N16" s="157">
+      <c r="N16" s="199">
         <v>0.98399999999999999</v>
       </c>
-      <c r="O16" s="2"/>
-      <c r="P16" s="169">
+      <c r="O16" s="192"/>
+      <c r="P16" s="247">
         <v>0.997</v>
       </c>
       <c r="Q16" s="32"/>
       <c r="R16" s="32"/>
     </row>
-    <row r="17" spans="1:18" ht="14.7" thickBot="1">
+    <row r="17" spans="1:18" ht="15.75" thickBot="1">
       <c r="A17" s="32"/>
-      <c r="B17" s="173"/>
+      <c r="B17" s="157"/>
       <c r="C17" s="119">
         <v>4</v>
       </c>
-      <c r="D17" s="158">
+      <c r="D17" s="221">
         <v>0.997</v>
       </c>
-      <c r="E17" s="159">
+      <c r="E17" s="222">
         <v>0.997</v>
       </c>
-      <c r="F17" s="160">
+      <c r="F17" s="223">
         <v>0.99199999999999999</v>
       </c>
-      <c r="G17" s="161">
+      <c r="G17" s="224">
         <v>0.99399999999999999</v>
       </c>
-      <c r="H17" s="162">
+      <c r="H17" s="225">
         <v>0.99099999999999999</v>
       </c>
-      <c r="I17" s="163">
+      <c r="I17" s="199">
         <v>0.98299999999999998</v>
       </c>
-      <c r="J17" s="164">
+      <c r="J17" s="199">
         <v>0.98199999999999998</v>
       </c>
-      <c r="K17" s="165">
+      <c r="K17" s="199">
         <v>0.97799999999999998</v>
       </c>
-      <c r="L17" s="165">
+      <c r="L17" s="226">
         <v>0.99</v>
       </c>
-      <c r="M17" s="165">
+      <c r="M17" s="199">
         <v>0.98899999999999999</v>
       </c>
-      <c r="N17" s="166">
+      <c r="N17" s="199">
         <v>0.98299999999999998</v>
       </c>
-      <c r="O17" s="2"/>
-      <c r="P17" s="170">
+      <c r="O17" s="192"/>
+      <c r="P17" s="248">
         <v>1</v>
       </c>
       <c r="Q17" s="32"/>
@@ -2987,7 +3383,7 @@
       <c r="Q18" s="32"/>
       <c r="R18" s="32"/>
     </row>
-    <row r="19" spans="1:18" ht="14.7" thickBot="1">
+    <row r="19" spans="1:18" ht="15.75" thickBot="1">
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
@@ -3007,58 +3403,58 @@
       <c r="Q19" s="32"/>
       <c r="R19" s="32"/>
     </row>
-    <row r="20" spans="1:18" ht="28" customHeight="1" thickBot="1">
+    <row r="20" spans="1:18" ht="27.95" customHeight="1" thickBot="1">
       <c r="A20" s="32"/>
-      <c r="B20" s="174" t="s">
+      <c r="B20" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="175"/>
-      <c r="D20" s="175"/>
-      <c r="E20" s="175"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="175"/>
-      <c r="H20" s="175"/>
-      <c r="I20" s="175"/>
-      <c r="J20" s="175"/>
-      <c r="K20" s="175"/>
-      <c r="L20" s="175"/>
-      <c r="M20" s="175"/>
-      <c r="N20" s="176"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="159"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="159"/>
+      <c r="G20" s="159"/>
+      <c r="H20" s="159"/>
+      <c r="I20" s="159"/>
+      <c r="J20" s="159"/>
+      <c r="K20" s="159"/>
+      <c r="L20" s="159"/>
+      <c r="M20" s="159"/>
+      <c r="N20" s="160"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="177" t="s">
+      <c r="P20" s="161" t="s">
         <v>11</v>
       </c>
       <c r="Q20" s="32"/>
       <c r="R20" s="32"/>
     </row>
-    <row r="21" spans="1:18" ht="14.7" thickBot="1">
+    <row r="21" spans="1:18" ht="15.75" thickBot="1">
       <c r="A21" s="32"/>
-      <c r="B21" s="180" t="s">
+      <c r="B21" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="181"/>
-      <c r="D21" s="184" t="s">
+      <c r="C21" s="165"/>
+      <c r="D21" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="185"/>
-      <c r="F21" s="185"/>
-      <c r="G21" s="185"/>
-      <c r="H21" s="185"/>
-      <c r="I21" s="185"/>
-      <c r="J21" s="185"/>
-      <c r="K21" s="185"/>
-      <c r="L21" s="185"/>
-      <c r="M21" s="185"/>
-      <c r="N21" s="186"/>
+      <c r="E21" s="169"/>
+      <c r="F21" s="169"/>
+      <c r="G21" s="169"/>
+      <c r="H21" s="169"/>
+      <c r="I21" s="169"/>
+      <c r="J21" s="169"/>
+      <c r="K21" s="169"/>
+      <c r="L21" s="169"/>
+      <c r="M21" s="169"/>
+      <c r="N21" s="170"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="178"/>
+      <c r="P21" s="162"/>
       <c r="Q21" s="32"/>
       <c r="R21" s="32"/>
     </row>
-    <row r="22" spans="1:18" ht="14.7" thickBot="1">
+    <row r="22" spans="1:18" ht="15.75" thickBot="1">
       <c r="A22" s="32"/>
-      <c r="B22" s="182"/>
-      <c r="C22" s="183"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="167"/>
       <c r="D22" s="118">
         <v>10</v>
       </c>
@@ -3093,53 +3489,53 @@
         <v>20</v>
       </c>
       <c r="O22" s="1"/>
-      <c r="P22" s="179"/>
+      <c r="P22" s="162"/>
       <c r="Q22" s="32"/>
       <c r="R22" s="32"/>
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1">
       <c r="A23" s="32"/>
-      <c r="B23" s="171" t="s">
+      <c r="B23" s="155" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="118">
         <v>1</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="199">
         <v>0.98499999999999999</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="227">
         <v>0.99099999999999999</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="228">
         <v>0.99399999999999999</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="229">
         <v>0.99299999999999999</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="230">
         <v>0.99299999999999999</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="231">
         <v>0.99399999999999999</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="232">
         <v>0.99199999999999999</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="233">
         <v>0.99399999999999999</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="234">
         <v>0.995</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="199">
         <v>0.98699999999999999</v>
       </c>
-      <c r="N23" s="155">
+      <c r="N23" s="235">
         <v>0.99</v>
       </c>
       <c r="O23" s="2"/>
-      <c r="P23" s="167">
+      <c r="P23" s="245">
         <v>0.99</v>
       </c>
       <c r="Q23" s="32"/>
@@ -3147,45 +3543,45 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="32"/>
-      <c r="B24" s="172"/>
+      <c r="B24" s="156"/>
       <c r="C24" s="116">
         <v>2</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="236">
         <v>0.99299999999999999</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="237">
         <v>0.996</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="12">
         <v>0.995</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="238">
         <v>0.99299999999999999</v>
       </c>
-      <c r="H24" s="17">
+      <c r="H24" s="239">
         <v>0.99199999999999999</v>
       </c>
-      <c r="I24" s="18">
+      <c r="I24" s="199">
         <v>0.98399999999999999</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="199">
         <v>0.98899999999999999</v>
       </c>
-      <c r="K24" s="20">
+      <c r="K24" s="230">
         <v>0.99299999999999999</v>
       </c>
-      <c r="L24" s="21">
+      <c r="L24" s="223">
         <v>0.99199999999999999</v>
       </c>
-      <c r="M24" s="22">
+      <c r="M24" s="240">
         <v>0.99299999999999999</v>
       </c>
-      <c r="N24" s="156">
+      <c r="N24" s="241">
         <v>0.99199999999999999</v>
       </c>
       <c r="O24" s="2"/>
-      <c r="P24" s="168">
+      <c r="P24" s="246">
         <v>0.99299999999999999</v>
       </c>
       <c r="Q24" s="32"/>
@@ -3193,91 +3589,91 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="32"/>
-      <c r="B25" s="172"/>
+      <c r="B25" s="156"/>
       <c r="C25" s="116">
         <v>3</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="199">
         <v>0.98599999999999999</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="199">
         <v>0.98299999999999998</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="237">
         <v>0.996</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="199">
         <v>0.98799999999999999</v>
       </c>
-      <c r="H25" s="26">
+      <c r="H25" s="199">
         <v>0.98399999999999999</v>
       </c>
-      <c r="I25" s="27">
+      <c r="I25" s="199">
         <v>0.98</v>
       </c>
-      <c r="J25" s="28">
+      <c r="J25" s="242">
         <v>0.99199999999999999</v>
       </c>
-      <c r="K25" s="29">
+      <c r="K25" s="243">
         <v>0.99199999999999999</v>
       </c>
-      <c r="L25" s="30">
+      <c r="L25" s="199">
         <v>0.98799999999999999</v>
       </c>
-      <c r="M25" s="31">
+      <c r="M25" s="199">
         <v>0.98599999999999999</v>
       </c>
-      <c r="N25" s="157">
+      <c r="N25" s="199">
         <v>0.98799999999999999</v>
       </c>
       <c r="O25" s="2"/>
-      <c r="P25" s="169">
+      <c r="P25" s="247">
         <v>0.997</v>
       </c>
       <c r="Q25" s="32"/>
       <c r="R25" s="32"/>
     </row>
-    <row r="26" spans="1:18" ht="14.7" thickBot="1">
+    <row r="26" spans="1:18" ht="15.75" thickBot="1">
       <c r="A26" s="32"/>
-      <c r="B26" s="173"/>
+      <c r="B26" s="157"/>
       <c r="C26" s="119">
         <v>4</v>
       </c>
-      <c r="D26" s="158">
+      <c r="D26" s="199">
         <v>0.98099999999999998</v>
       </c>
-      <c r="E26" s="159">
+      <c r="E26" s="244">
         <v>0.99</v>
       </c>
-      <c r="F26" s="160">
+      <c r="F26" s="199">
         <v>0.97499999999999998</v>
       </c>
-      <c r="G26" s="161">
+      <c r="G26" s="199">
         <v>0.92800000000000005</v>
       </c>
-      <c r="H26" s="162">
+      <c r="H26" s="199">
         <v>0.95099999999999996</v>
       </c>
-      <c r="I26" s="163">
+      <c r="I26" s="199">
         <v>0.98599999999999999</v>
       </c>
-      <c r="J26" s="164">
+      <c r="J26" s="199">
         <v>0.98499999999999999</v>
       </c>
-      <c r="K26" s="165">
+      <c r="K26" s="199">
         <v>0.98599999999999999</v>
       </c>
-      <c r="L26" s="165">
+      <c r="L26" s="199">
         <v>0.98599999999999999</v>
       </c>
-      <c r="M26" s="165">
+      <c r="M26" s="199">
         <v>0.98199999999999998</v>
       </c>
-      <c r="N26" s="166">
+      <c r="N26" s="199">
         <v>0.98499999999999999</v>
       </c>
       <c r="O26" s="2"/>
-      <c r="P26" s="170">
+      <c r="P26" s="248">
         <v>1</v>
       </c>
       <c r="Q26" s="32"/>
@@ -3337,96 +3733,6 @@
     <mergeCell ref="B21:C22"/>
     <mergeCell ref="D21:N21"/>
   </mergeCells>
-  <conditionalFormatting sqref="V16">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:N8">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="num" val="0.99"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="num" val="0.99"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:P8 D14:P17 D23:P26">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14:N17">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="num" val="0.99"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="num" val="0.99"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23:N26">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="0.99"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0.99"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3436,18 +3742,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B0A384-BA79-4C34-9B6A-E46A00C40AA1}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:P35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.68359375" customWidth="1"/>
-    <col min="15" max="15" width="3.83984375" customWidth="1"/>
-    <col min="16" max="16" width="9.15625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="3.85546875" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.7" thickBot="1">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1">
       <c r="A1" s="32"/>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -3467,58 +3773,58 @@
       <c r="Q1" s="32"/>
       <c r="R1" s="32"/>
     </row>
-    <row r="2" spans="1:18" ht="28" customHeight="1" thickBot="1">
+    <row r="2" spans="1:18" ht="27.95" customHeight="1" thickBot="1">
       <c r="A2" s="32"/>
-      <c r="B2" s="194" t="s">
+      <c r="B2" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="195"/>
-      <c r="L2" s="195"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="196"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="172"/>
+      <c r="H2" s="172"/>
+      <c r="I2" s="172"/>
+      <c r="J2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
+      <c r="M2" s="172"/>
+      <c r="N2" s="173"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="177" t="s">
+      <c r="P2" s="161" t="s">
         <v>13</v>
       </c>
       <c r="Q2" s="32"/>
       <c r="R2" s="32"/>
     </row>
-    <row r="3" spans="1:18" ht="14.7" thickBot="1">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1">
       <c r="A3" s="32"/>
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="207" t="s">
+      <c r="C3" s="175"/>
+      <c r="D3" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="202"/>
-      <c r="J3" s="202"/>
-      <c r="K3" s="202"/>
-      <c r="L3" s="202"/>
-      <c r="M3" s="202"/>
-      <c r="N3" s="203"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
+      <c r="N3" s="180"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="178"/>
+      <c r="P3" s="162"/>
       <c r="Q3" s="32"/>
       <c r="R3" s="32"/>
     </row>
-    <row r="4" spans="1:18" ht="14.7" thickBot="1">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1">
       <c r="A4" s="32"/>
-      <c r="B4" s="199"/>
-      <c r="C4" s="200"/>
+      <c r="B4" s="176"/>
+      <c r="C4" s="177"/>
       <c r="D4" s="118">
         <v>10</v>
       </c>
@@ -3553,13 +3859,13 @@
         <v>20</v>
       </c>
       <c r="O4" s="1"/>
-      <c r="P4" s="179"/>
+      <c r="P4" s="163"/>
       <c r="Q4" s="32"/>
       <c r="R4" s="32"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" ht="15" customHeight="1">
       <c r="A5" s="32"/>
-      <c r="B5" s="204" t="s">
+      <c r="B5" s="181" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="118">
@@ -3598,7 +3904,7 @@
       <c r="N5" s="143">
         <v>1.1299999999999999</v>
       </c>
-      <c r="O5" s="42"/>
+      <c r="O5" s="249"/>
       <c r="P5" s="125">
         <v>0</v>
       </c>
@@ -3607,7 +3913,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="32"/>
-      <c r="B6" s="205"/>
+      <c r="B6" s="182"/>
       <c r="C6" s="116">
         <v>2</v>
       </c>
@@ -3644,7 +3950,7 @@
       <c r="N6" s="144">
         <v>1.77</v>
       </c>
-      <c r="O6" s="42"/>
+      <c r="O6" s="249"/>
       <c r="P6" s="126">
         <v>10</v>
       </c>
@@ -3653,7 +3959,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="32"/>
-      <c r="B7" s="205"/>
+      <c r="B7" s="182"/>
       <c r="C7" s="116">
         <v>3</v>
       </c>
@@ -3690,16 +3996,16 @@
       <c r="N7" s="145">
         <v>3.57</v>
       </c>
-      <c r="O7" s="42"/>
+      <c r="O7" s="249"/>
       <c r="P7" s="127">
         <v>100</v>
       </c>
       <c r="Q7" s="32"/>
       <c r="R7" s="32"/>
     </row>
-    <row r="8" spans="1:18" ht="14.7" thickBot="1">
+    <row r="8" spans="1:18" ht="15.75" thickBot="1">
       <c r="A8" s="32"/>
-      <c r="B8" s="206"/>
+      <c r="B8" s="183"/>
       <c r="C8" s="119">
         <v>4</v>
       </c>
@@ -3736,7 +4042,7 @@
       <c r="N8" s="154">
         <v>2.9</v>
       </c>
-      <c r="O8" s="42"/>
+      <c r="O8" s="249"/>
       <c r="P8" s="128">
         <v>600</v>
       </c>
@@ -3763,7 +4069,7 @@
       <c r="Q9" s="32"/>
       <c r="R9" s="32"/>
     </row>
-    <row r="10" spans="1:18" ht="14.7" thickBot="1">
+    <row r="10" spans="1:18" ht="15.75" thickBot="1">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
@@ -3783,58 +4089,58 @@
       <c r="Q10" s="32"/>
       <c r="R10" s="32"/>
     </row>
-    <row r="11" spans="1:18" ht="28" customHeight="1" thickBot="1">
+    <row r="11" spans="1:18" ht="27.95" customHeight="1" thickBot="1">
       <c r="A11" s="32"/>
-      <c r="B11" s="194" t="s">
+      <c r="B11" s="171" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="195"/>
-      <c r="D11" s="195"/>
-      <c r="E11" s="195"/>
-      <c r="F11" s="195"/>
-      <c r="G11" s="195"/>
-      <c r="H11" s="195"/>
-      <c r="I11" s="195"/>
-      <c r="J11" s="195"/>
-      <c r="K11" s="195"/>
-      <c r="L11" s="195"/>
-      <c r="M11" s="195"/>
-      <c r="N11" s="196"/>
+      <c r="C11" s="172"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="172"/>
+      <c r="F11" s="172"/>
+      <c r="G11" s="172"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="172"/>
+      <c r="J11" s="172"/>
+      <c r="K11" s="172"/>
+      <c r="L11" s="172"/>
+      <c r="M11" s="172"/>
+      <c r="N11" s="173"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="177" t="s">
+      <c r="P11" s="161" t="s">
         <v>14</v>
       </c>
       <c r="Q11" s="32"/>
       <c r="R11" s="32"/>
     </row>
-    <row r="12" spans="1:18" ht="14.7" thickBot="1">
+    <row r="12" spans="1:18" ht="15.75" thickBot="1">
       <c r="A12" s="32"/>
-      <c r="B12" s="197" t="s">
+      <c r="B12" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="198"/>
-      <c r="D12" s="207" t="s">
+      <c r="C12" s="175"/>
+      <c r="D12" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="202"/>
-      <c r="F12" s="202"/>
-      <c r="G12" s="202"/>
-      <c r="H12" s="202"/>
-      <c r="I12" s="202"/>
-      <c r="J12" s="202"/>
-      <c r="K12" s="202"/>
-      <c r="L12" s="202"/>
-      <c r="M12" s="202"/>
-      <c r="N12" s="203"/>
+      <c r="E12" s="179"/>
+      <c r="F12" s="179"/>
+      <c r="G12" s="179"/>
+      <c r="H12" s="179"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="179"/>
+      <c r="K12" s="179"/>
+      <c r="L12" s="179"/>
+      <c r="M12" s="179"/>
+      <c r="N12" s="180"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="178"/>
+      <c r="P12" s="162"/>
       <c r="Q12" s="32"/>
       <c r="R12" s="32"/>
     </row>
-    <row r="13" spans="1:18" ht="14.7" thickBot="1">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1">
       <c r="A13" s="32"/>
-      <c r="B13" s="199"/>
-      <c r="C13" s="200"/>
+      <c r="B13" s="176"/>
+      <c r="C13" s="177"/>
       <c r="D13" s="118">
         <v>10</v>
       </c>
@@ -3869,13 +4175,13 @@
         <v>20</v>
       </c>
       <c r="O13" s="1"/>
-      <c r="P13" s="179"/>
+      <c r="P13" s="163"/>
       <c r="Q13" s="32"/>
       <c r="R13" s="32"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="32"/>
-      <c r="B14" s="204" t="s">
+      <c r="B14" s="181" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="118">
@@ -3923,7 +4229,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="32"/>
-      <c r="B15" s="205"/>
+      <c r="B15" s="182"/>
       <c r="C15" s="116">
         <v>2</v>
       </c>
@@ -3969,7 +4275,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="32"/>
-      <c r="B16" s="205"/>
+      <c r="B16" s="182"/>
       <c r="C16" s="116">
         <v>3</v>
       </c>
@@ -4013,9 +4319,9 @@
       <c r="Q16" s="32"/>
       <c r="R16" s="32"/>
     </row>
-    <row r="17" spans="1:18" ht="14.7" thickBot="1">
+    <row r="17" spans="1:18" ht="15.75" thickBot="1">
       <c r="A17" s="32"/>
-      <c r="B17" s="206"/>
+      <c r="B17" s="183"/>
       <c r="C17" s="119">
         <v>4</v>
       </c>
@@ -4064,63 +4370,63 @@
       <c r="Q18" s="32"/>
       <c r="R18" s="32"/>
     </row>
-    <row r="19" spans="1:18" ht="14.7" thickBot="1">
+    <row r="19" spans="1:18" ht="15.75" thickBot="1">
       <c r="A19" s="32"/>
       <c r="Q19" s="32"/>
       <c r="R19" s="32"/>
     </row>
-    <row r="20" spans="1:18" ht="28" customHeight="1" thickBot="1">
+    <row r="20" spans="1:18" ht="27.95" customHeight="1" thickBot="1">
       <c r="A20" s="32"/>
-      <c r="B20" s="187" t="s">
+      <c r="B20" s="185" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="188"/>
-      <c r="D20" s="188"/>
-      <c r="E20" s="188"/>
-      <c r="F20" s="188"/>
-      <c r="G20" s="188"/>
-      <c r="H20" s="188"/>
-      <c r="I20" s="188"/>
-      <c r="J20" s="188"/>
-      <c r="K20" s="188"/>
-      <c r="L20" s="188"/>
-      <c r="M20" s="188"/>
-      <c r="N20" s="189"/>
+      <c r="C20" s="186"/>
+      <c r="D20" s="186"/>
+      <c r="E20" s="186"/>
+      <c r="F20" s="186"/>
+      <c r="G20" s="186"/>
+      <c r="H20" s="186"/>
+      <c r="I20" s="186"/>
+      <c r="J20" s="186"/>
+      <c r="K20" s="186"/>
+      <c r="L20" s="186"/>
+      <c r="M20" s="186"/>
+      <c r="N20" s="187"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="177" t="s">
+      <c r="P20" s="161" t="s">
         <v>14</v>
       </c>
       <c r="Q20" s="32"/>
       <c r="R20" s="32"/>
     </row>
-    <row r="21" spans="1:18" ht="14.7" thickBot="1">
+    <row r="21" spans="1:18" ht="15.75" thickBot="1">
       <c r="A21" s="32"/>
-      <c r="B21" s="190" t="s">
+      <c r="B21" s="188" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="191"/>
-      <c r="D21" s="184" t="s">
+      <c r="C21" s="189"/>
+      <c r="D21" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="185"/>
-      <c r="F21" s="185"/>
-      <c r="G21" s="185"/>
-      <c r="H21" s="185"/>
-      <c r="I21" s="185"/>
-      <c r="J21" s="185"/>
-      <c r="K21" s="185"/>
-      <c r="L21" s="185"/>
-      <c r="M21" s="185"/>
-      <c r="N21" s="186"/>
+      <c r="E21" s="169"/>
+      <c r="F21" s="169"/>
+      <c r="G21" s="169"/>
+      <c r="H21" s="169"/>
+      <c r="I21" s="169"/>
+      <c r="J21" s="169"/>
+      <c r="K21" s="169"/>
+      <c r="L21" s="169"/>
+      <c r="M21" s="169"/>
+      <c r="N21" s="170"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="178"/>
+      <c r="P21" s="162"/>
       <c r="Q21" s="32"/>
       <c r="R21" s="32"/>
     </row>
-    <row r="22" spans="1:18" ht="14.7" thickBot="1">
+    <row r="22" spans="1:18" ht="15.75" thickBot="1">
       <c r="A22" s="32"/>
-      <c r="B22" s="192"/>
-      <c r="C22" s="193"/>
+      <c r="B22" s="190"/>
+      <c r="C22" s="191"/>
       <c r="D22" s="118">
         <v>10</v>
       </c>
@@ -4155,13 +4461,13 @@
         <v>20</v>
       </c>
       <c r="O22" s="1"/>
-      <c r="P22" s="179"/>
+      <c r="P22" s="163"/>
       <c r="Q22" s="32"/>
       <c r="R22" s="32"/>
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1">
       <c r="A23" s="32"/>
-      <c r="B23" s="171" t="s">
+      <c r="B23" s="155" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="118">
@@ -4209,7 +4515,7 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="32"/>
-      <c r="B24" s="172"/>
+      <c r="B24" s="156"/>
       <c r="C24" s="116">
         <v>2</v>
       </c>
@@ -4255,7 +4561,7 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="32"/>
-      <c r="B25" s="172"/>
+      <c r="B25" s="156"/>
       <c r="C25" s="116">
         <v>3</v>
       </c>
@@ -4299,9 +4605,9 @@
       <c r="Q25" s="32"/>
       <c r="R25" s="32"/>
     </row>
-    <row r="26" spans="1:18" ht="14.7" thickBot="1">
+    <row r="26" spans="1:18" ht="15.75" thickBot="1">
       <c r="A26" s="32"/>
-      <c r="B26" s="173"/>
+      <c r="B26" s="157"/>
       <c r="C26" s="119">
         <v>4</v>
       </c>
@@ -4363,7 +4669,7 @@
       <c r="P27" s="32"/>
       <c r="Q27" s="32"/>
     </row>
-    <row r="28" spans="1:18" ht="14.7" thickBot="1">
+    <row r="28" spans="1:18" ht="15.75" thickBot="1">
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
       <c r="D28" s="32"/>
@@ -4381,51 +4687,51 @@
       <c r="P28" s="32"/>
       <c r="Q28" s="32"/>
     </row>
-    <row r="29" spans="1:18" ht="28" customHeight="1" thickBot="1">
-      <c r="B29" s="194" t="s">
+    <row r="29" spans="1:18" ht="27.95" customHeight="1" thickBot="1">
+      <c r="B29" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="195"/>
-      <c r="D29" s="195"/>
-      <c r="E29" s="195"/>
-      <c r="F29" s="195"/>
-      <c r="G29" s="195"/>
-      <c r="H29" s="195"/>
-      <c r="I29" s="195"/>
-      <c r="J29" s="195"/>
-      <c r="K29" s="195"/>
-      <c r="L29" s="195"/>
-      <c r="M29" s="195"/>
-      <c r="N29" s="196"/>
+      <c r="C29" s="172"/>
+      <c r="D29" s="172"/>
+      <c r="E29" s="172"/>
+      <c r="F29" s="172"/>
+      <c r="G29" s="172"/>
+      <c r="H29" s="172"/>
+      <c r="I29" s="172"/>
+      <c r="J29" s="172"/>
+      <c r="K29" s="172"/>
+      <c r="L29" s="172"/>
+      <c r="M29" s="172"/>
+      <c r="N29" s="173"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="177" t="s">
+      <c r="P29" s="161" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="14.7" thickBot="1">
-      <c r="B30" s="197" t="s">
+    <row r="30" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B30" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="198"/>
-      <c r="D30" s="201" t="s">
+      <c r="C30" s="175"/>
+      <c r="D30" s="184" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="202"/>
-      <c r="F30" s="202"/>
-      <c r="G30" s="202"/>
-      <c r="H30" s="202"/>
-      <c r="I30" s="202"/>
-      <c r="J30" s="202"/>
-      <c r="K30" s="202"/>
-      <c r="L30" s="202"/>
-      <c r="M30" s="202"/>
-      <c r="N30" s="203"/>
+      <c r="E30" s="179"/>
+      <c r="F30" s="179"/>
+      <c r="G30" s="179"/>
+      <c r="H30" s="179"/>
+      <c r="I30" s="179"/>
+      <c r="J30" s="179"/>
+      <c r="K30" s="179"/>
+      <c r="L30" s="179"/>
+      <c r="M30" s="179"/>
+      <c r="N30" s="180"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="178"/>
-    </row>
-    <row r="31" spans="1:18" ht="14.7" thickBot="1">
-      <c r="B31" s="199"/>
-      <c r="C31" s="200"/>
+      <c r="P30" s="162"/>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B31" s="176"/>
+      <c r="C31" s="177"/>
       <c r="D31" s="118">
         <v>10</v>
       </c>
@@ -4460,10 +4766,10 @@
         <v>20</v>
       </c>
       <c r="O31" s="1"/>
-      <c r="P31" s="179"/>
+      <c r="P31" s="163"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1">
-      <c r="B32" s="204" t="s">
+      <c r="B32" s="181" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="118">
@@ -4508,7 +4814,7 @@
       </c>
     </row>
     <row r="33" spans="2:16">
-      <c r="B33" s="205"/>
+      <c r="B33" s="182"/>
       <c r="C33" s="116">
         <v>2</v>
       </c>
@@ -4551,7 +4857,7 @@
       </c>
     </row>
     <row r="34" spans="2:16">
-      <c r="B34" s="205"/>
+      <c r="B34" s="182"/>
       <c r="C34" s="116">
         <v>3</v>
       </c>
@@ -4593,8 +4899,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="2:16" ht="14.7" thickBot="1">
-      <c r="B35" s="206"/>
+    <row r="35" spans="2:16" ht="15.75" thickBot="1">
+      <c r="B35" s="183"/>
       <c r="C35" s="119">
         <v>4</v>
       </c>
@@ -4672,75 +4978,27 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B20:N20"/>
+    <mergeCell ref="D21:N21"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="P20:P22"/>
+    <mergeCell ref="B29:N29"/>
+    <mergeCell ref="P29:P31"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="D30:N30"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B11:N11"/>
+    <mergeCell ref="P11:P13"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="D12:N12"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="P2:P4"/>
     <mergeCell ref="B3:C4"/>
     <mergeCell ref="D3:N3"/>
     <mergeCell ref="B5:B8"/>
-    <mergeCell ref="B11:N11"/>
-    <mergeCell ref="P11:P13"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="D12:N12"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B29:N29"/>
-    <mergeCell ref="P29:P31"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="D30:N30"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B20:N20"/>
-    <mergeCell ref="D21:N21"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="P20:P22"/>
   </mergeCells>
-  <conditionalFormatting sqref="V16">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O14:P17">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:P8 D23:P26 D32:P35">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32:P35 D23:P26 D14:P17 D5:P8">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>